<commit_message>
Sd corrections questionnaire (#344)
* correction code PS => P01

* changement placement binding

* add pour questionnaire dans les capability statements

* correction SP CS

* changement type de slice pour useContext

* correction warning sushi exemple

* correction slicing 91d17fd56d0e61fc05eae5eed3cb6e8465643841
</commit_message>
<xml_diff>
--- a/main/ig/ValueSet-ror-usage-context-type-vs.xlsx
+++ b/main/ig/ValueSet-ror-usage-context-type-vs.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-22T16:25:12+00:00</t>
+    <t>2024-04-02T15:41:03+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension du Value Set http://hl7.org/fhir/ValueSet/usage-context-type pour fixer le type de contexte d'usage de la fiche de saisie avec le code EG ou le S pour Spécialité ordinale</t>
+    <t>Extension du Value Set http://hl7.org/fhir/ValueSet/usage-context-type pour fixer le type de contexte d'usage de la fiche de saisie avec le code EG ou le S pour Spécialité ordinale ou P01 pour le type de profession</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -129,7 +129,7 @@
     <t>https://mos.esante.gouv.fr/NOS/TRE_R04-TypeSavoirFaire/FHIR/TRE-R04-TypeSavoirFaire</t>
   </si>
   <si>
-    <t>PS</t>
+    <t>P01</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/TRE_R288-TypeProfession/FHIR/TRE-R288-TypeProfession</t>

</xml_diff>